<commit_message>
tmple excel upload data
</commit_message>
<xml_diff>
--- a/template excel uploaad/upload excel.xlsx
+++ b/template excel uploaad/upload excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\SiJak-21-LLDikti-III\template excel uploaad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Backup\UNINDRAKu\magang\MSIB Batch 5\LLDIKTI III\Aplikasi Pajak SiJak\template excel uploaad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75A2747-B065-47F4-8A64-BFBA83C0937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F1B8EE-576F-4CCF-94EA-C277D97A7965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-3915" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3495" yWindow="4185" windowWidth="19905" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upload excel" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>no_H01</t>
   </si>
@@ -141,9 +141,6 @@
     <t>status_pegawai</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
     <t>VI/a</t>
   </si>
   <si>
@@ -171,37 +168,16 @@
     <t>atas_ph_23B</t>
   </si>
   <si>
-    <t>Himsar Silaban</t>
-  </si>
-  <si>
-    <t>195303071975081001</t>
-  </si>
-  <si>
-    <t>0001</t>
-  </si>
-  <si>
-    <t>2024-01-01</t>
-  </si>
-  <si>
-    <t>1989-05-21</t>
-  </si>
-  <si>
-    <t>2024-02-01</t>
-  </si>
-  <si>
-    <t>2023-04-01</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>Acep</t>
+  </si>
+  <si>
+    <t>Ucup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -706,9 +682,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1066,396 +1042,397 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AK5" sqref="AK5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.54296875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.08984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="1"/>
-    <col min="7" max="7" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.1796875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="7.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="37" width="21.1796875" style="1" customWidth="1"/>
-    <col min="38" max="38" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="37" width="21.140625" customWidth="1"/>
+    <col min="38" max="38" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="12" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK1" t="s">
         <v>44</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45020</v>
+      </c>
+      <c r="D2">
+        <v>123123</v>
+      </c>
+      <c r="E2">
+        <v>1230912</v>
+      </c>
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>35</v>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1">
+        <v>36922</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1234570000000000</v>
+      </c>
+      <c r="L2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2">
+        <v>1000000</v>
+      </c>
+      <c r="O2">
+        <v>300000</v>
+      </c>
+      <c r="P2">
+        <v>15000</v>
+      </c>
+      <c r="Q2">
+        <v>1035150</v>
+      </c>
+      <c r="R2">
+        <v>240000</v>
+      </c>
+      <c r="S2">
+        <v>123132</v>
+      </c>
+      <c r="T2">
+        <v>1000</v>
+      </c>
+      <c r="U2">
+        <v>120031</v>
+      </c>
+      <c r="V2">
+        <v>1312218</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>131230</v>
+      </c>
+      <c r="Y2">
+        <v>13913129</v>
+      </c>
+      <c r="Z2">
+        <v>109310391</v>
+      </c>
+      <c r="AA2">
+        <v>121320</v>
+      </c>
+      <c r="AB2">
+        <v>132412</v>
+      </c>
+      <c r="AC2">
+        <v>123123</v>
+      </c>
+      <c r="AD2">
+        <v>123123</v>
+      </c>
+      <c r="AE2">
+        <v>12391</v>
+      </c>
+      <c r="AF2">
+        <v>1023910</v>
+      </c>
+      <c r="AG2">
+        <v>123123</v>
+      </c>
+      <c r="AH2">
+        <v>131321</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ2">
+        <v>21</v>
+      </c>
+      <c r="AK2">
+        <v>12</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="1">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C3" s="1">
+        <v>45020</v>
+      </c>
+      <c r="D3">
+        <v>321321</v>
+      </c>
+      <c r="E3">
+        <v>1230912</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1">
+        <v>36922</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1234570000000000</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3">
+        <v>1000000</v>
+      </c>
+      <c r="O3">
+        <v>300000</v>
+      </c>
+      <c r="P3">
+        <v>15000</v>
+      </c>
+      <c r="Q3">
+        <v>1035150</v>
+      </c>
+      <c r="R3">
+        <v>240000</v>
+      </c>
+      <c r="S3">
+        <v>123132</v>
+      </c>
+      <c r="T3">
+        <v>1000</v>
+      </c>
+      <c r="U3">
+        <v>120031</v>
+      </c>
+      <c r="V3">
+        <v>1312218</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>131230</v>
+      </c>
+      <c r="Y3">
+        <v>13913129</v>
+      </c>
+      <c r="Z3">
+        <v>109310391</v>
+      </c>
+      <c r="AA3">
+        <v>121320</v>
+      </c>
+      <c r="AB3">
+        <v>132412</v>
+      </c>
+      <c r="AC3">
         <v>123123</v>
       </c>
-      <c r="E2" s="1">
-        <v>1230912</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1234570000000000</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="AD3">
+        <v>123123</v>
+      </c>
+      <c r="AE3">
+        <v>12391</v>
+      </c>
+      <c r="AF3">
+        <v>1023910</v>
+      </c>
+      <c r="AG3">
+        <v>123123</v>
+      </c>
+      <c r="AH3">
+        <v>131321</v>
+      </c>
+      <c r="AI3" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="O2" s="1">
-        <v>300000</v>
-      </c>
-      <c r="P2" s="1">
-        <v>15000</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>1035150</v>
-      </c>
-      <c r="R2" s="1">
-        <v>240000</v>
-      </c>
-      <c r="S2" s="1">
-        <v>123132</v>
-      </c>
-      <c r="T2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="U2" s="1">
-        <v>120031</v>
-      </c>
-      <c r="V2" s="1">
-        <v>1312218</v>
-      </c>
-      <c r="W2" s="1">
-        <v>0</v>
-      </c>
-      <c r="X2" s="1">
-        <v>131230</v>
-      </c>
-      <c r="Y2" s="1">
-        <v>13913129</v>
-      </c>
-      <c r="Z2" s="1">
-        <v>109310391</v>
-      </c>
-      <c r="AA2" s="1">
-        <v>121320</v>
-      </c>
-      <c r="AB2" s="1">
-        <v>132412</v>
-      </c>
-      <c r="AC2" s="1">
-        <v>123123</v>
-      </c>
-      <c r="AD2" s="1">
-        <v>123123</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>12391</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>1023910</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>123123</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>131321</v>
-      </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ3">
+        <v>21</v>
+      </c>
+      <c r="AK3">
+        <v>12</v>
+      </c>
+      <c r="AL3" t="s">
         <v>41</v>
-      </c>
-      <c r="AJ2" s="1">
-        <v>21</v>
-      </c>
-      <c r="AK2" s="1">
-        <v>12</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2000000001</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="1">
-        <v>688861822432000</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1234570000000000</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
-        <v>22646899</v>
-      </c>
-      <c r="O3" s="1">
-        <v>2264680</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>24911579</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
-        <v>5400147</v>
-      </c>
-      <c r="T3" s="1">
-        <v>579360</v>
-      </c>
-      <c r="U3" s="1">
-        <v>30891086</v>
-      </c>
-      <c r="V3" s="1">
-        <v>0</v>
-      </c>
-      <c r="W3" s="1">
-        <v>691667</v>
-      </c>
-      <c r="X3" s="1">
-        <v>31582753</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1579133</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>1494133</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>3073266</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>28509487</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>85528461</v>
-      </c>
-      <c r="AE3" s="1">
-        <v>27028000</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>450466</v>
-      </c>
-      <c r="AG3" s="1">
-        <v>223345</v>
-      </c>
-      <c r="AH3" s="1">
-        <v>450466</v>
-      </c>
-      <c r="AI3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>